<commit_message>
choice changes in sheet
</commit_message>
<xml_diff>
--- a/media/delegates_round1.xlsx
+++ b/media/delegates_round1.xlsx
@@ -6409,33 +6409,32 @@
   </sheetPr>
   <dimension ref="A1:Z265"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H251" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E260" activeCellId="0" sqref="E260"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N259" activeCellId="0" sqref="N259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="51.969387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="49.6785714285714"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="35.6377551020408"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="38.4744897959184"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="98.545918367347"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="46.4387755102041"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="31.4540816326531"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="66.8214285714286"/>
-    <col collapsed="false" hidden="false" max="17" min="15" style="0" width="43.469387755102"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="66.8214285714286"/>
-    <col collapsed="false" hidden="false" max="21" min="19" style="0" width="43.469387755102"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="66.8214285714286"/>
-    <col collapsed="false" hidden="false" max="25" min="23" style="0" width="43.469387755102"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="91.6581632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="51.4336734693878"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="49.1377551020408"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="35.0969387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="37.9336734693878"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="97.4642857142857"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="45.8979591836735"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="31.0459183673469"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="66.0102040816327"/>
+    <col collapsed="false" hidden="false" max="17" min="15" style="0" width="42.9285714285714"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="66.0102040816327"/>
+    <col collapsed="false" hidden="false" max="21" min="19" style="0" width="42.9285714285714"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="66.0102040816327"/>
+    <col collapsed="false" hidden="false" max="25" min="23" style="0" width="42.9285714285714"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="90.7142857142857"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26712,31 +26711,31 @@
         <v>0</v>
       </c>
       <c r="M258" s="0" t="s">
-        <v>1628</v>
+        <v>271</v>
       </c>
       <c r="N258" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="O258" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="P258" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q258" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="R258" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="O258" s="0" t="s">
+      <c r="S258" s="0" t="s">
         <v>96</v>
-      </c>
-      <c r="P258" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q258" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="R258" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="S258" s="0" t="s">
-        <v>202</v>
       </c>
       <c r="T258" s="0" t="s">
         <v>72</v>
       </c>
       <c r="U258" s="0" t="s">
-        <v>251</v>
+        <v>69</v>
       </c>
       <c r="V258" s="0" t="s">
         <v>42</v>

</xml_diff>